<commit_message>
everything works for now
</commit_message>
<xml_diff>
--- a/IceElemental/ExcelReports/Write/Furniture2007.xlsx
+++ b/IceElemental/ExcelReports/Write/Furniture2007.xlsx
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +403,7 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>ARONChair</t>
+          <t>IKEAChair</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
@@ -413,12 +413,12 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>60</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>600</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Pesho</t>
+          <t>IKEABed</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
@@ -440,12 +440,12 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>15.5</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>806</t>
+          <t>6240</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Pesho</t>
+          <t>ARONMirror</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
@@ -467,12 +467,12 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>432</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Pesho</t>
+          <t>VidenovChair</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>ARONMirror</t>
+          <t>ARONChair</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
@@ -521,12 +521,147 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>70</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>280</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Sunset Security</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>IKEAMirror</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>280</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>West Bank</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ARONChair</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>1400</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>BILLA</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>ARONBed</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>2550</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>Null Industries</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>IKEABed</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>2520</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>VS Incorporated</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>IKEAMirror</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>140</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
there was some error that we fixed
</commit_message>
<xml_diff>
--- a/IceElemental/ExcelReports/Write/Furniture2007.xlsx
+++ b/IceElemental/ExcelReports/Write/Furniture2007.xlsx
@@ -370,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="G6" sqref="G6"/>
@@ -3635,6 +3635,276 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="122">
+      <c r="A122" s="0" t="inlineStr">
+        <is>
+          <t>AIKO</t>
+        </is>
+      </c>
+      <c r="B122" s="0" t="inlineStr">
+        <is>
+          <t>ARON Unicorn Toilet</t>
+        </is>
+      </c>
+      <c r="C122" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D122" s="0" t="inlineStr">
+        <is>
+          <t>106.47</t>
+        </is>
+      </c>
+      <c r="E122" s="0" t="inlineStr">
+        <is>
+          <t>1064.7</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="123">
+      <c r="A123" s="0" t="inlineStr">
+        <is>
+          <t>Telerik Academy</t>
+        </is>
+      </c>
+      <c r="B123" s="0" t="inlineStr">
+        <is>
+          <t>IKEA Dendroid Chair</t>
+        </is>
+      </c>
+      <c r="C123" s="0" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="D123" s="0" t="inlineStr">
+        <is>
+          <t>73.8</t>
+        </is>
+      </c>
+      <c r="E123" s="0" t="inlineStr">
+        <is>
+          <t>3837.6</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="124">
+      <c r="A124" s="0" t="inlineStr">
+        <is>
+          <t>Boyana Film Studios</t>
+        </is>
+      </c>
+      <c r="B124" s="0" t="inlineStr">
+        <is>
+          <t>ARON Medusa Mirror</t>
+        </is>
+      </c>
+      <c r="C124" s="0" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D124" s="0" t="inlineStr">
+        <is>
+          <t>52.74</t>
+        </is>
+      </c>
+      <c r="E124" s="0" t="inlineStr">
+        <is>
+          <t>1265.76</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="125">
+      <c r="A125" s="0" t="inlineStr">
+        <is>
+          <t>San Benedetto</t>
+        </is>
+      </c>
+      <c r="B125" s="0" t="inlineStr">
+        <is>
+          <t>IKEA Medusa Mirror</t>
+        </is>
+      </c>
+      <c r="C125" s="0" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D125" s="0" t="inlineStr">
+        <is>
+          <t>36.95</t>
+        </is>
+      </c>
+      <c r="E125" s="0" t="inlineStr">
+        <is>
+          <t>295.6</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="126">
+      <c r="A126" s="0" t="inlineStr">
+        <is>
+          <t>Mladost Estate</t>
+        </is>
+      </c>
+      <c r="B126" s="0" t="inlineStr">
+        <is>
+          <t>ARON Dendroid Chair</t>
+        </is>
+      </c>
+      <c r="C126" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D126" s="0" t="inlineStr">
+        <is>
+          <t>213.85</t>
+        </is>
+      </c>
+      <c r="E126" s="0" t="inlineStr">
+        <is>
+          <t>855.4</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="127">
+      <c r="A127" s="0" t="inlineStr">
+        <is>
+          <t>Sunset Security</t>
+        </is>
+      </c>
+      <c r="B127" s="0" t="inlineStr">
+        <is>
+          <t>ARON Vampire Lamp</t>
+        </is>
+      </c>
+      <c r="C127" s="0" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D127" s="0" t="inlineStr">
+        <is>
+          <t>86.16</t>
+        </is>
+      </c>
+      <c r="E127" s="0" t="inlineStr">
+        <is>
+          <t>1206.24</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="128">
+      <c r="A128" s="0" t="inlineStr">
+        <is>
+          <t>West Bank</t>
+        </is>
+      </c>
+      <c r="B128" s="0" t="inlineStr">
+        <is>
+          <t>ARON Dendroid Chair</t>
+        </is>
+      </c>
+      <c r="C128" s="0" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D128" s="0" t="inlineStr">
+        <is>
+          <t>213.85</t>
+        </is>
+      </c>
+      <c r="E128" s="0" t="inlineStr">
+        <is>
+          <t>4277</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="129">
+      <c r="A129" s="0" t="inlineStr">
+        <is>
+          <t>BILLA</t>
+        </is>
+      </c>
+      <c r="B129" s="0" t="inlineStr">
+        <is>
+          <t>ARON Zombie Bed</t>
+        </is>
+      </c>
+      <c r="C129" s="0" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D129" s="0" t="inlineStr">
+        <is>
+          <t>193.05</t>
+        </is>
+      </c>
+      <c r="E129" s="0" t="inlineStr">
+        <is>
+          <t>3281.85</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="130">
+      <c r="A130" s="0" t="inlineStr">
+        <is>
+          <t>Null Industries</t>
+        </is>
+      </c>
+      <c r="B130" s="0" t="inlineStr">
+        <is>
+          <t>IKEA Dendroid Chair</t>
+        </is>
+      </c>
+      <c r="C130" s="0" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D130" s="0" t="inlineStr">
+        <is>
+          <t>73.8</t>
+        </is>
+      </c>
+      <c r="E130" s="0" t="inlineStr">
+        <is>
+          <t>1549.8</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="131">
+      <c r="A131" s="0" t="inlineStr">
+        <is>
+          <t>VS Incorporated</t>
+        </is>
+      </c>
+      <c r="B131" s="0" t="inlineStr">
+        <is>
+          <t>ARON Vampire Lamp</t>
+        </is>
+      </c>
+      <c r="C131" s="0" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D131" s="0" t="inlineStr">
+        <is>
+          <t>86.16</t>
+        </is>
+      </c>
+      <c r="E131" s="0" t="inlineStr">
+        <is>
+          <t>603.12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>